<commit_message>
Add Grand Total in Accounting Sales Report ref: http://dev.netforce.com/online/helpdesk-support/issues/162
</commit_message>
<xml_diff>
--- a/netforce_account_report/netforce_account_report/reports/account_sale.xlsx
+++ b/netforce_account_report/netforce_account_report/reports/account_sale.xlsx
@@ -5,73 +5,84 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="240" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
-  <si>
-    <t>Accounting Sales Report</t>
-  </si>
-  <si>
-    <t>{{company_name}}</t>
-  </si>
-  <si>
-    <t>From {{fmt_date date_from}} to {{fmt_date date_to}}</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Account</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>{{#each groups}}</t>
-  </si>
-  <si>
-    <t>{{contact_name}}</t>
-  </si>
-  <si>
-    <t>{{#each lines}}</t>
-  </si>
-  <si>
-    <t>{{number}}</t>
-  </si>
-  <si>
-    <t>{{date}}</t>
-  </si>
-  <si>
-    <t>{{description}}</t>
-  </si>
-  <si>
-    <t>[{{account_code}}] {{account_name}}</t>
-  </si>
-  <si>
-    <t>{{currency amount}}</t>
-  </si>
-  <si>
-    <t>{{/each}}</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>{{currency total}}</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+  <si>
+    <t xml:space="preserve">Accounting Sales Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{company_name}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From {{fmt_date date_from}} to {{fmt_date date_to}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{#each groups}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{contact_name}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{#each lines}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{number}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{date}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{description}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{{account_code}}] {{account_name}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency amount}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{/each}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency total}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency grand_total}}</t>
   </si>
 </sst>
 </file>
@@ -79,7 +90,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -327,35 +338,35 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.515306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.6785714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.2040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.0102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0255102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.5765306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.7142857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.1326530612245"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.2397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.68367346938776"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E1" s="2"/>
     </row>
-    <row r="2" s="1" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -367,7 +378,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" s="1" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -379,7 +390,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" s="1" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -465,13 +476,25 @@
         <v>16</v>
       </c>
     </row>
+    <row r="14" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="3">
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:H4"/>
-    <mergeCell ref="5:5"/>
-    <mergeCell ref="8:8"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>